<commit_message>
daily_tasks 테이블에 insert할 sql 예시(찬영)
</commit_message>
<xml_diff>
--- a/DB레코드.xlsx
+++ b/DB레코드.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{39B23785-F77B-4074-9BD5-B9362C04CFE6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15760" windowHeight="4530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="4536" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="매뉴얼" sheetId="1" r:id="rId1"/>
     <sheet name="일일업무" sheetId="2" r:id="rId2"/>
+    <sheet name="DB Insert용" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">일일업무!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">일일업무!$A$1:$D$35</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="138">
   <si>
     <t>위생관리</t>
   </si>
@@ -457,45 +461,145 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>미들</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일일업무 데이터 넣을 때 설정하는 것
-** 완료자아이디 &amp; 완료자명 없을 수 있다
-** 중요업무여부 0, 1 (알아서 설정)
-** 직접입력업무 1개씩
-** 오픈, 미들, 마감, 개인업무 2~3개씩
-배정날짜 DATE
-(아래는 약식)
-2018/05/06 ~ 07  - 찬영
-2018/05/08 ~ 09  - 태훈
-2018/05/10 ~ 11  - 윤석
-지점코드 branch_seq 는 1 (매장 하나임)
-완료자 아이디 / 완료자 명
-yunseok / 장윤석
-chanyoung / 주찬영
-taehun / 김태훈
-yunyoung / 홍윤영
-yunjin / 김연진
-// 매뉴얼업무코드 not null -&gt; null 변경
-alter table daily_tasks modify manual_tasks_seq number(5) null;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공간분류 
  insert into space_types(space_types_seq, space_type) values(space_types_seq.nextval, '홀');
  insert into space_types(space_types_seq, space_type) values(space_types_seq.nextval, '바');
  insert into space_types(space_types_seq, space_type) values(space_types_seq.nextval, '카운터');
  insert into space_types(space_types_seq, space_type) values(space_types_seq.nextval, '테라스');
  insert into space_types(space_types_seq, space_type) values(space_types_seq.nextval, '화장실');</t>
+  </si>
+  <si>
+    <t>미들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>daily_tasks_seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assign_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>input_task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>importance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assign_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assign_detail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매뉴얼업무코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>manual_tasks_seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finisher_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finisher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch_seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>daily_tasks_seq.nextval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018/05/06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yunjin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김연진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yunyoung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018/05/07</t>
+  </si>
+  <si>
+    <t>파라솔 상태 점검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yunseok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chanyoung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>taehun</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>assigner_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주찬영</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장윤석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김태훈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오픈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마감</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>찬영SQL문</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -521,12 +625,21 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -535,7 +648,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -547,6 +660,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -861,23 +980,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="30.4140625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.9140625" customWidth="1"/>
-    <col min="6" max="6" width="148.4140625" customWidth="1"/>
-    <col min="7" max="7" width="76.25" customWidth="1"/>
+    <col min="3" max="3" width="30.3984375" customWidth="1"/>
+    <col min="4" max="4" width="11.69921875" customWidth="1"/>
+    <col min="5" max="5" width="11.8984375" customWidth="1"/>
+    <col min="6" max="6" width="148.3984375" customWidth="1"/>
+    <col min="7" max="7" width="76.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -894,7 +1013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="167.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="167.55" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -905,13 +1024,13 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -931,7 +1050,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -945,7 +1064,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -962,7 +1081,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -976,7 +1095,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -993,7 +1112,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
         <v>28</v>
       </c>
@@ -1007,7 +1126,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -1024,7 +1143,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
         <v>26</v>
       </c>
@@ -1038,7 +1157,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1058,7 +1177,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>63</v>
@@ -1073,7 +1192,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1209,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
         <v>34</v>
       </c>
@@ -1098,7 +1217,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -1115,7 +1234,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="C16" t="s">
         <v>36</v>
       </c>
@@ -1129,7 +1248,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -1140,7 +1259,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C18" t="s">
         <v>37</v>
       </c>
@@ -1148,7 +1267,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1168,7 +1287,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>82</v>
@@ -1183,7 +1302,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1319,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C22" s="3" t="s">
         <v>85</v>
       </c>
@@ -1214,7 +1333,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -1231,7 +1350,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C24" s="3" t="s">
         <v>88</v>
       </c>
@@ -1245,7 +1364,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -1258,7 +1377,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C26" s="3" t="s">
         <v>91</v>
       </c>
@@ -1268,7 +1387,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1288,7 +1407,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
         <v>44</v>
       </c>
@@ -1302,7 +1421,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -1319,7 +1438,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C30" t="s">
         <v>47</v>
       </c>
@@ -1327,7 +1446,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1347,7 +1466,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C32" t="s">
         <v>49</v>
       </c>
@@ -1361,7 +1480,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -1378,7 +1497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="C34" t="s">
         <v>51</v>
       </c>
@@ -1392,7 +1511,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B35" t="s">
         <v>23</v>
       </c>
@@ -1409,7 +1528,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
       <c r="C36" t="s">
         <v>103</v>
       </c>
@@ -1425,21 +1544,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34A8806-9519-42B2-8BC4-39A19318EE5A}">
-  <dimension ref="A1:C39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.4140625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.9140625" customWidth="1"/>
+    <col min="1" max="1" width="30.3984375" customWidth="1"/>
+    <col min="2" max="2" width="11.69921875" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" customWidth="1"/>
+    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1449,30 +1570,39 @@
       <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1482,186 +1612,219 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>62</v>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="3" t="s">
-        <v>82</v>
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>43</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>53</v>
       </c>
       <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
         <v>54</v>
@@ -1669,19 +1832,25 @@
       <c r="C21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>88</v>
       </c>
@@ -1691,32 +1860,33 @@
       <c r="C23" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="D23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
         <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>50</v>
       </c>
       <c r="B26" t="s">
         <v>42</v>
@@ -1724,87 +1894,986 @@
       <c r="C26" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34">
         <v>33</v>
       </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    </row>
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45"/>
-    <row r="39" spans="1:3" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="3" t="s">
-        <v>106</v>
-      </c>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{E6DF14E8-3CC0-4E25-AF95-FE471687BBC3}">
-    <sortState ref="A2:C36">
-      <sortCondition ref="C1"/>
+  <autoFilter ref="A1:D35">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="기간"/>
+      </filters>
+    </filterColumn>
+    <sortState ref="A2:D35">
+      <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H2" s="1">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="1">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="1">
+        <v>29</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H9" s="1">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="1">
+        <v>19</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="1">
+        <v>22</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" s="1">
+        <v>25</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="1">
+        <v>31</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H14" s="1">
+        <v>17</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="B16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="1">
+        <v>11</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H18" s="1">
+        <v>8</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="1">
+        <v>32</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H20" s="1">
+        <v>6</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="1">
+        <v>13</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="1">
+        <v>20</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="G24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="G25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
daily_tasks 담당 파트 insert 쿼리문 작성
</commit_message>
<xml_diff>
--- a/DB레코드.xlsx
+++ b/DB레코드.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{60B544A9-A7EC-4792-9834-9E6502985BC5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15756" windowHeight="4536" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="4530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="매뉴얼" sheetId="1" r:id="rId1"/>
     <sheet name="일일업무" sheetId="2" r:id="rId2"/>
     <sheet name="DB Insert용" sheetId="3" r:id="rId3"/>
+    <sheet name="daily_tasks_query" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">일일업무!$A$1:$D$35</definedName>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="224">
   <si>
     <t>위생관리</t>
   </si>
@@ -595,11 +597,340 @@
     <t>찬영SQL문</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>태훈sql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,</t>
+  </si>
+  <si>
+    <t>'파트',</t>
+  </si>
+  <si>
+    <t>'오픈',</t>
+  </si>
+  <si>
+    <t>null,</t>
+  </si>
+  <si>
+    <t>'yunyoung',</t>
+  </si>
+  <si>
+    <t>TO_DATE('2018-05-08','YYYY-MM-DD'),</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DAILY_TASKS_seq.nextval,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레몬청 만들기',</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TO_DATE('2018-05-09','YYYY-MM-DD'),</t>
+  </si>
+  <si>
+    <t>TO_DATE('2018-05-10','YYYY-MM-DD'),</t>
+  </si>
+  <si>
+    <t>1,</t>
+  </si>
+  <si>
+    <t>'마감'</t>
+  </si>
+  <si>
+    <t>'미들'</t>
+  </si>
+  <si>
+    <t>2,</t>
+  </si>
+  <si>
+    <t>3,</t>
+  </si>
+  <si>
+    <t>4,</t>
+  </si>
+  <si>
+    <t>5,</t>
+  </si>
+  <si>
+    <t>6,</t>
+  </si>
+  <si>
+    <t>7,</t>
+  </si>
+  <si>
+    <t>8,</t>
+  </si>
+  <si>
+    <t>9,</t>
+  </si>
+  <si>
+    <t>10,</t>
+  </si>
+  <si>
+    <t>11,</t>
+  </si>
+  <si>
+    <t>12,</t>
+  </si>
+  <si>
+    <t>13,</t>
+  </si>
+  <si>
+    <t>'yunseok',</t>
+  </si>
+  <si>
+    <t>'장윤석',</t>
+  </si>
+  <si>
+    <t>'주찬영',</t>
+  </si>
+  <si>
+    <t>'taehun',</t>
+  </si>
+  <si>
+    <t>'김태훈',</t>
+  </si>
+  <si>
+    <t>'yunjin',</t>
+  </si>
+  <si>
+    <t>'김연진',</t>
+  </si>
+  <si>
+    <t>'chanyoung',</t>
+  </si>
+  <si>
+    <t>1,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14,</t>
+  </si>
+  <si>
+    <t>15,</t>
+  </si>
+  <si>
+    <t>17,</t>
+  </si>
+  <si>
+    <t>18,</t>
+  </si>
+  <si>
+    <t>19,</t>
+  </si>
+  <si>
+    <t>20,</t>
+  </si>
+  <si>
+    <t>21,</t>
+  </si>
+  <si>
+    <t>22,</t>
+  </si>
+  <si>
+    <t>24,</t>
+  </si>
+  <si>
+    <t>25,</t>
+  </si>
+  <si>
+    <t>26,</t>
+  </si>
+  <si>
+    <t>27,</t>
+  </si>
+  <si>
+    <t>28,</t>
+  </si>
+  <si>
+    <t>29,</t>
+  </si>
+  <si>
+    <t>신메뉴 팝업 제작',</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보건증 갱신'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'개인',</t>
+  </si>
+  <si>
+    <t>1);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, '레몬청 만들기', TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '개인', 'yunseok', null, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '파트', '오픈', 1, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '파트', '오픈', 2, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '개인', 'yunjin', 3, 'yunjin', '김연진', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '파트', '미들', 4, 'yunjin', '김연진', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '파트', '미들', 5, 'yunjin', '김연진', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ)
+ values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '개인', 'taehun', 6, 'taehun', '김태훈', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '파트', '마감', 7, 'taehun', '김태훈', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '파트', '마감', 8, 'taehun', '김태훈', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '개인', 'taehun', 9, 'taehun', '김태훈', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '파트', '오픈', 10, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '파트', '오픈', 11, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '파트', '오픈', 12, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '파트', '미들', 13, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '파트', '미들', 14, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '파트', '미들', 15, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, '보건증 갱신', TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '개인', 'yunseok', null, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '파트', '마감', 17, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '파트', '마감', 18, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '개인', ''chanyoung', 19, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '파트', '오픈', 20, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '파트', '오픈', 21, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '파트', '오픈', 22, 'taehun', '김태훈', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ)  
+values(DAILY_TASKS_seq.nextval, '신메뉴 팝업 제작', TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '개인', 'taehun', null, 'taehun', '김태훈', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '개인', 'chanyoung', 24, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '파트', '미들', 26, 'yunjin', '김연진', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '파트', '미들', 25, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '파트', '마감', 27, null, null, 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '파트', '마감', 28, null, null, 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '개인', 'yunjin', 29, null, null, 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태훈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>daily_tasks 데이터 추가용 쿼리문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -625,7 +956,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -642,13 +973,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -665,6 +1014,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -980,23 +1350,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30.3984375" customWidth="1"/>
-    <col min="4" max="4" width="11.69921875" customWidth="1"/>
-    <col min="5" max="5" width="11.8984375" customWidth="1"/>
-    <col min="6" max="6" width="148.3984375" customWidth="1"/>
-    <col min="7" max="7" width="76.19921875" customWidth="1"/>
+    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="6" max="6" width="148.375" customWidth="1"/>
+    <col min="7" max="7" width="76.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="167.55" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="167.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1030,7 +1400,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1050,7 +1420,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -1064,7 +1434,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +1451,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -1095,7 +1465,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -1112,7 +1482,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>28</v>
       </c>
@@ -1126,7 +1496,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -1143,7 +1513,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>26</v>
       </c>
@@ -1157,7 +1527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1177,7 +1547,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>63</v>
@@ -1192,7 +1562,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -1209,7 +1579,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>34</v>
       </c>
@@ -1217,7 +1587,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -1234,7 +1604,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>36</v>
       </c>
@@ -1248,7 +1618,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -1259,7 +1629,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>37</v>
       </c>
@@ -1267,7 +1637,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1287,7 +1657,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>82</v>
@@ -1302,7 +1672,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1689,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
         <v>85</v>
       </c>
@@ -1333,7 +1703,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -1350,7 +1720,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
         <v>88</v>
       </c>
@@ -1364,7 +1734,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -1377,7 +1747,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
         <v>91</v>
       </c>
@@ -1387,7 +1757,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1407,7 +1777,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>44</v>
       </c>
@@ -1421,7 +1791,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -1438,7 +1808,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>47</v>
       </c>
@@ -1446,7 +1816,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1466,7 +1836,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>49</v>
       </c>
@@ -1480,7 +1850,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -1497,7 +1867,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>51</v>
       </c>
@@ -1511,7 +1881,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>23</v>
       </c>
@@ -1528,7 +1898,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>103</v>
       </c>
@@ -1544,23 +1914,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.3984375" customWidth="1"/>
-    <col min="2" max="2" width="11.69921875" customWidth="1"/>
-    <col min="3" max="3" width="11.8984375" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.375" customWidth="1"/>
+    <col min="2" max="2" width="11.75" customWidth="1"/>
+    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1944,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1588,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1602,7 +1972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1616,7 +1986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1630,7 +2000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1644,7 +2014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1658,7 +2028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1672,7 +2042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1686,7 +2056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>62</v>
       </c>
@@ -1700,7 +2070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>63</v>
       </c>
@@ -1714,7 +2084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1728,7 +2098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1736,7 +2106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1750,7 +2120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1764,7 +2134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -1772,7 +2142,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1780,7 +2150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -1794,7 +2164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>82</v>
       </c>
@@ -1808,7 +2178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>59</v>
       </c>
@@ -1822,7 +2192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>85</v>
       </c>
@@ -1836,7 +2206,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>57</v>
       </c>
@@ -1850,7 +2220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>88</v>
       </c>
@@ -1864,7 +2234,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>61</v>
       </c>
@@ -1874,7 +2244,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>91</v>
       </c>
@@ -1884,7 +2254,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1898,7 +2268,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1912,7 +2282,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -1926,7 +2296,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1934,7 +2304,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -1948,7 +2318,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -1962,7 +2332,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1976,7 +2346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -1990,7 +2360,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -2004,7 +2374,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -2012,11 +2382,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D35">
+  <autoFilter ref="A1:D35" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="1">
       <filters>
         <filter val="기간"/>
@@ -2033,30 +2403,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9" style="1"/>
+    <col min="15" max="15" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>107</v>
       </c>
@@ -2091,8 +2463,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>137</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2129,7 +2501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>118</v>
       </c>
@@ -2164,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>118</v>
       </c>
@@ -2199,7 +2571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>118</v>
       </c>
@@ -2234,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>118</v>
       </c>
@@ -2269,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>118</v>
       </c>
@@ -2304,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>118</v>
       </c>
@@ -2339,7 +2711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>118</v>
       </c>
@@ -2374,7 +2746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>118</v>
       </c>
@@ -2409,7 +2781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>118</v>
       </c>
@@ -2444,7 +2816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>118</v>
       </c>
@@ -2479,7 +2851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>118</v>
       </c>
@@ -2514,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>118</v>
       </c>
@@ -2549,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>118</v>
       </c>
@@ -2584,7 +2956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>118</v>
       </c>
@@ -2619,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>118</v>
       </c>
@@ -2654,7 +3026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>118</v>
       </c>
@@ -2689,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>118</v>
       </c>
@@ -2724,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>118</v>
       </c>
@@ -2759,7 +3131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>118</v>
       </c>
@@ -2794,7 +3166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>118</v>
       </c>
@@ -2829,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>118</v>
       </c>
@@ -2864,16 +3236,1251 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="G24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="G25" s="1"/>
-      <c r="I25" s="1"/>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B31" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B33" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B37" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B39" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B40" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B41" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B42" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B43" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B45" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B46" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B47" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B48" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L48" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B49" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L49" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B50" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L50" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B51" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L51" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B52" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B53" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K54" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="L54" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAFB34E-2FEC-4B7C-B013-1E0F4A147F5F}">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="182.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B15" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B17" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B18" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B25" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
모델링 수정, finisher -> finisher_name sql문 모두 수정
</commit_message>
<xml_diff>
--- a/DB레코드.xlsx
+++ b/DB레코드.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{60B544A9-A7EC-4792-9834-9E6502985BC5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEFBA9A-13EF-4A88-ABAC-2C75DAC37455}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="4530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15760" windowHeight="4530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="매뉴얼" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="226">
   <si>
     <t>위생관리</t>
   </si>
@@ -507,14 +507,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>finisher_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>finisher</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>branch_seq</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -617,10 +609,6 @@
     <t>'yunyoung',</t>
   </si>
   <si>
-    <t>TO_DATE('2018-05-08','YYYY-MM-DD'),</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DAILY_TASKS_seq.nextval,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -629,12 +617,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TO_DATE('2018-05-09','YYYY-MM-DD'),</t>
-  </si>
-  <si>
-    <t>TO_DATE('2018-05-10','YYYY-MM-DD'),</t>
-  </si>
-  <si>
     <t>1,</t>
   </si>
   <si>
@@ -769,161 +751,158 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, '레몬청 만들기', TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '개인', 'yunseok', null, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '파트', '오픈', 1, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '파트', '오픈', 2, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '개인', 'yunjin', 3, 'yunjin', '김연진', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '파트', '미들', 4, 'yunjin', '김연진', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '파트', '미들', 5, 'yunjin', '김연진', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ)
- values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '개인', 'taehun', 6, 'taehun', '김태훈', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '파트', '마감', 7, 'taehun', '김태훈', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 0, '파트', '마감', 8, 'taehun', '김태훈', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-08','YYYY-MM-DD'), 1, '개인', 'taehun', 9, 'taehun', '김태훈', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '파트', '오픈', 10, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '파트', '오픈', 11, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '파트', '오픈', 12, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '파트', '미들', 13, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '파트', '미들', 14, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '파트', '미들', 15, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, '보건증 갱신', TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '개인', 'yunseok', null, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '파트', '마감', 17, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 0, '파트', '마감', 18, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-09','YYYY-MM-DD'), 1, '개인', ''chanyoung', 19, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '파트', '오픈', 20, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '파트', '오픈', 21, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '파트', '오픈', 22, 'taehun', '김태훈', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ)  
-values(DAILY_TASKS_seq.nextval, '신메뉴 팝업 제작', TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '개인', 'taehun', null, 'taehun', '김태훈', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '개인', 'chanyoung', 24, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '파트', '미들', 26, 'yunjin', '김연진', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '파트', '미들', 25, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '파트', '마감', 27, null, null, 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 0, '파트', '마감', 28, null, null, 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, TO_DATE('2018-05-10','YYYY-MM-DD'), 1, '개인', 'yunjin', 29, null, null, 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>태훈</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>daily_tasks 데이터 추가용 쿼리문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤석SQL문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018/05/11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, '레몬청 만들기',  '2018/05/08', 0, '개인', 'yunseok', null, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '파트', '오픈', 1, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '개인', 'yunjin', 3, 'yunjin', '김연진', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '파트', '미들', 4, 'yunjin', '김연진', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '파트', '미들', 5, 'yunjin', '김연진', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ)
+ values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '개인', 'taehun', 6, 'taehun', '김태훈', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '파트', '마감', 7, 'taehun', '김태훈', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '파트', '마감', 8, 'taehun', '김태훈', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '개인', 'taehun', 9, 'taehun', '김태훈', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 0, '파트', '오픈', 10, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '파트', '오픈', 11, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 0, '파트', '오픈', 12, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '파트', '미들', 13, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 0, '파트', '미들', 14, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '파트', '미들', 15, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, '보건증 갱신', '2018/05/09', 0, '개인', 'yunseok', null, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '파트', '마감', 17, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 0, '파트', '마감', 18, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '개인', ''chanyoung', 19, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 0, '파트', '오픈', 20, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '파트', '오픈', 21, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '파트', '오픈', 22, 'taehun', '김태훈', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ)  
+values(DAILY_TASKS_seq.nextval, '신메뉴 팝업 제작', '2018/05/10', 0, '개인', 'taehun', null, 'taehun', '김태훈', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '개인', 'chanyoung', 24, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '파트', '미들', 25, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 0, '파트', '미들', 26, 'yunjin', '김연진', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 0, '파트', '마감', 27, null, null, 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 0, '파트', '마감', 28, null, null, 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '개인', 'yunjin', 29, null, null, 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>finisher_name_id</t>
+  </si>
+  <si>
+    <t>finisher_name</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '파트', '오픈', 2, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연진이 피카츄 생일케이크 사오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근무태만 반성문 작성해오기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -997,7 +976,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1035,6 +1014,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1357,16 +1345,16 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="5" width="11.875" customWidth="1"/>
-    <col min="6" max="6" width="148.375" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="148.33203125" customWidth="1"/>
     <col min="7" max="7" width="76.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1383,7 +1371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="167.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="167.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1400,7 +1388,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1420,7 +1408,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>16</v>
       </c>
@@ -1434,7 +1422,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -1451,7 +1439,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -1465,7 +1453,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -1482,7 +1470,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C8" t="s">
         <v>28</v>
       </c>
@@ -1496,7 +1484,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -1513,7 +1501,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>26</v>
       </c>
@@ -1527,7 +1515,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1547,7 +1535,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>63</v>
@@ -1562,7 +1550,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -1579,7 +1567,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>34</v>
       </c>
@@ -1587,7 +1575,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -1604,7 +1592,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>36</v>
       </c>
@@ -1618,7 +1606,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>23</v>
       </c>
@@ -1629,7 +1617,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>37</v>
       </c>
@@ -1637,7 +1625,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1657,7 +1645,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>82</v>
@@ -1672,7 +1660,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -1689,7 +1677,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C22" s="3" t="s">
         <v>85</v>
       </c>
@@ -1703,7 +1691,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -1720,7 +1708,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C24" s="3" t="s">
         <v>88</v>
       </c>
@@ -1734,7 +1722,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>39</v>
       </c>
@@ -1747,7 +1735,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C26" s="3" t="s">
         <v>91</v>
       </c>
@@ -1757,7 +1745,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1777,7 +1765,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
         <v>44</v>
       </c>
@@ -1791,7 +1779,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -1808,7 +1796,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
         <v>47</v>
       </c>
@@ -1816,7 +1804,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1836,7 +1824,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
         <v>49</v>
       </c>
@@ -1850,7 +1838,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>1</v>
       </c>
@@ -1867,7 +1855,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
         <v>51</v>
       </c>
@@ -1881,7 +1869,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>23</v>
       </c>
@@ -1898,7 +1886,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
         <v>103</v>
       </c>
@@ -1915,22 +1903,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.375" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.75" customWidth="1"/>
-    <col min="3" max="3" width="11.875" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1944,7 +1931,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1958,7 +1945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1972,7 +1959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1986,7 +1973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2000,7 +1987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -2014,7 +2001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2028,7 +2015,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2042,7 +2029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2056,7 +2043,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>62</v>
       </c>
@@ -2070,7 +2057,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>63</v>
       </c>
@@ -2084,7 +2071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -2098,7 +2085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -2106,7 +2093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -2120,7 +2107,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2134,7 +2121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -2142,7 +2129,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2150,7 +2137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>60</v>
       </c>
@@ -2164,7 +2151,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>82</v>
       </c>
@@ -2178,7 +2165,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>59</v>
       </c>
@@ -2192,7 +2179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>85</v>
       </c>
@@ -2206,7 +2193,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>57</v>
       </c>
@@ -2220,7 +2207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>88</v>
       </c>
@@ -2234,7 +2221,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>61</v>
       </c>
@@ -2244,7 +2231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>91</v>
       </c>
@@ -2254,7 +2241,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -2268,7 +2255,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -2282,7 +2269,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -2296,7 +2283,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -2304,7 +2291,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>97</v>
       </c>
@@ -2318,7 +2305,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2332,7 +2319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -2346,7 +2333,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -2360,7 +2347,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -2374,7 +2361,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>103</v>
       </c>
@@ -2382,20 +2369,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D35" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="기간"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:D35">
-      <sortCondition ref="D1"/>
-    </sortState>
-  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2404,31 +2381,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.75" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.75" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.25" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11.25" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="9" style="1"/>
-    <col min="15" max="15" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="4" t="s">
         <v>107</v>
       </c>
@@ -2451,30 +2429,30 @@
         <v>114</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -2483,33 +2461,33 @@
         <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H2" s="1">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="L2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -2518,33 +2496,33 @@
         <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -2553,33 +2531,33 @@
         <v>42</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H4" s="1">
         <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -2594,62 +2572,62 @@
         <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="H6" s="1">
         <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
@@ -2664,27 +2642,27 @@
         <v>29</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L7" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -2693,33 +2671,33 @@
         <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H8" s="1">
         <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -2728,33 +2706,33 @@
         <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H9" s="1">
         <v>10</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -2763,33 +2741,33 @@
         <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H10" s="1">
         <v>19</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L10" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -2798,33 +2776,33 @@
         <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H11" s="1">
         <v>22</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L11" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -2833,33 +2811,33 @@
         <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H12" s="1">
         <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L12" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B13" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>120</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -2868,33 +2846,33 @@
         <v>42</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H13" s="1">
         <v>31</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B14" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -2903,33 +2881,33 @@
         <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H14" s="1">
         <v>17</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B15" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -2938,33 +2916,33 @@
         <v>42</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H15" s="1">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="L15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B16" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -2973,33 +2951,33 @@
         <v>42</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H16" s="1">
         <v>4</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="L16" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B17" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
@@ -3014,62 +2992,62 @@
         <v>11</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L17" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B18" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="H18" s="1">
         <v>8</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L18" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B19" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -3084,27 +3062,27 @@
         <v>32</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L19" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -3113,33 +3091,33 @@
         <v>42</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H20" s="1">
         <v>6</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L20" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B21" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -3148,33 +3126,33 @@
         <v>42</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H21" s="1">
         <v>13</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L21" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B22" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E22" s="1">
         <v>1</v>
@@ -3183,33 +3161,33 @@
         <v>42</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H22" s="1">
         <v>20</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L22" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B23" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -3218,1092 +3196,1509 @@
         <v>42</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L23" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D25" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B26" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="G26" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B27" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B28" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B29" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B30" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D30" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B31" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B32" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D32" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="H32" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B33" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="13">
+        <v>43228</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B34" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="14">
+        <v>43228</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B35" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B36" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B37" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B38" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G38" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="H38" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B39" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D39" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B40" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D40" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F40" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B41" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D41" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B42" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K42" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B43" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="13">
+        <v>43229</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B44" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D44" s="14">
+        <v>43229</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="L44" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B45" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="15">
+        <v>43230</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="G25" s="11" t="s">
+      <c r="H45" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B46" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D46" s="13">
+        <v>43230</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="K46" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B47" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="13">
+        <v>43230</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J47" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K47" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L47" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B48" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D48" s="13">
+        <v>43230</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="J48" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="K48" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L48" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B49" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="13">
+        <v>43230</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J49" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K49" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L49" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B50" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D50" s="13">
+        <v>43230</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J50" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="K50" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L50" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B51" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D51" s="13">
+        <v>43230</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I51" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="J51" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L51" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B52" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="C52" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D52" s="13">
+        <v>43230</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="J52" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L52" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B53" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D53" s="13">
+        <v>43230</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I53" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B54" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="14">
+        <v>43230</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="G54" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F26" s="8" t="s">
+      <c r="H54" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="I54" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="J54" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="K54" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="H26" s="8" t="s">
-        <v>172</v>
-      </c>
-      <c r="I26" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L26" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="O27" s="6"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B28" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="O28" s="6"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B29" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B30" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B31" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="H31" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B32" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K32" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L32" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K33" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L33" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="L34" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B35" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="K36" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B37" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="I37" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B38" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H38" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L38" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B39" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H39" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K39" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L39" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B40" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L40" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B41" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B42" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="I42" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="J42" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="K42" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L42" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B43" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="H43" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="J43" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="K43" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="I44" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="K44" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="L44" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B45" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="I45" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="J45" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="L45" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B46" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H46" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="I46" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="J46" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="K46" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L46" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B47" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="J47" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K47" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L47" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B48" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="G48" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="H48" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I48" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="J48" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="K48" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L48" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B49" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="H49" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="I49" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="J49" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="K49" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L49" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B50" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H50" s="8" t="s">
-        <v>182</v>
-      </c>
-      <c r="I50" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="J50" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="K50" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L50" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B51" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="J51" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="K51" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L51" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B52" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="H52" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="I52" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J52" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="K52" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L52" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B53" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G53" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="H53" s="8" t="s">
+      <c r="L54" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="I53" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J53" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="K53" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L53" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="I54" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="J54" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="K54" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="L54" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H56" s="1">
+        <v>17</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E57" s="1">
+        <v>0</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H57" s="1">
+        <v>12</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B58" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H58" s="1">
+        <v>28</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B59" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H59" s="1">
+        <v>24</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B61" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H61" s="1">
+        <v>34</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B62" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E62" s="1">
+        <v>0</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H62" s="1">
+        <v>20</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B63" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H63" s="1">
+        <v>5</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="B64" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H64" s="1">
+        <v>19</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B65" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E65" s="1">
+        <v>0</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H65" s="1">
+        <v>16</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B66" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E66" s="1">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L66" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="D77" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4311,171 +4706,171 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAFB34E-2FEC-4B7C-B013-1E0F4A147F5F}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="182.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B5" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+    <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B7" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B8" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    <row r="9" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B9" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B10" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+    <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B11" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="12" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B12" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
+    <row r="13" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B13" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B14" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B14" s="3" t="s">
+    <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B15" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B15" s="3" t="s">
+    <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B16" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
+    <row r="17" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B17" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+    <row r="18" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B18" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+    <row r="19" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B19" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B19" s="3" t="s">
+    <row r="20" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B20" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
+    <row r="21" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B21" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
+    <row r="22" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B22" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B22" s="3" t="s">
+    <row r="23" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B23" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
+    <row r="24" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B24" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B24" s="3" t="s">
+    <row r="25" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B25" s="3" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B25" s="3" t="s">
+    <row r="26" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B26" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B26" s="3" t="s">
+    <row r="27" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B27" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B27" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="33" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B30" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
+    <row r="31" spans="2:2" ht="34" x14ac:dyDescent="0.45">
+      <c r="B31" s="3" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FINISHER_NAME_ID -> FINISHER_ID로 수정
</commit_message>
<xml_diff>
--- a/DB레코드.xlsx
+++ b/DB레코드.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4047D83-274E-4DFA-AE21-6E8E366ADFF5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC62F506-1145-4814-B533-2FCA158FF74E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="3690" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -767,172 +767,173 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>연진이 피카츄 생일케이크 사오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근무태만 반성문 작성해오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김연진</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>개인</t>
+  </si>
+  <si>
+    <t>오픈</t>
+  </si>
+  <si>
+    <t>yunjin</t>
+  </si>
+  <si>
+    <t>미들</t>
+  </si>
+  <si>
+    <t>yunseok</t>
+  </si>
+  <si>
+    <t>장윤석</t>
+  </si>
+  <si>
+    <t>마감</t>
+  </si>
+  <si>
+    <t>taehun</t>
+  </si>
+  <si>
+    <t>김태훈</t>
+  </si>
+  <si>
+    <t>finisher_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>finisher_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, '레몬청 만들기',  '2018/05/08', 0, '개인', 'yunseok', null, 'yunseok', '장윤석', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '파트', '오픈', 1, 'yunseok', '장윤석', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '파트', '오픈', 2, 'yunseok', '장윤석', 'yunyoung', 1)</t>
+  </si>
+  <si>
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '개인', 'yunjin', 3, 'yunjin', '김연진', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '파트', '미들', 4, 'yunjin', '김연진', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '파트', '미들', 5, 'yunjin', '김연진', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ)
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ)
  values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '개인', 'taehun', 6, 'taehun', '김태훈', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '파트', '마감', 7, 'taehun', '김태훈', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '파트', '마감', 8, 'taehun', '김태훈', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 1, '개인', 'taehun', 9, 'taehun', '김태훈', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 0, '파트', '오픈', 10, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '파트', '오픈', 11, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 0, '파트', '오픈', 12, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '파트', '미들', 13, 'yunseok', '장윤석', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 0, '파트', '미들', 14, 'yunseok', '장윤석', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '파트', '미들', 15, 'yunseok', '장윤석', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, '보건증 갱신', '2018/05/09', 0, '개인', 'yunseok', null, 'yunseok', '장윤석', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '파트', '마감', 17, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 0, '파트', '마감', 18, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/09', 1, '개인', ''chanyoung', 19, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 0, '파트', '오픈', 20, 'yunseok', '장윤석', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '파트', '오픈', 21, 'yunseok', '장윤석', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '파트', '오픈', 22, 'taehun', '김태훈', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ)  
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ)  
 values(DAILY_TASKS_seq.nextval, '신메뉴 팝업 제작', '2018/05/10', 0, '개인', 'taehun', null, 'taehun', '김태훈', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '개인', 'chanyoung', 24, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '파트', '미들', 25, 'chanyoung', '주찬영', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 0, '파트', '미들', 26, 'yunjin', '김연진', 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 0, '파트', '마감', 27, null, null, 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 0, '파트', '마감', 28, null, null, 'yunyoung', 1)</t>
   </si>
   <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
+    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
 values(DAILY_TASKS_seq.nextval, null, '2018/05/10', 1, '개인', 'yunjin', 29, null, null, 'yunyoung', 1)</t>
-  </si>
-  <si>
-    <t>finisher_name_id</t>
-  </si>
-  <si>
-    <t>finisher_name</t>
-  </si>
-  <si>
-    <t>insert into daily_tasks (DAILY_TASKS_SEQ, INPUT_TASK, ASSIGN_DATE, IMPORTANCE, ASSIGN_TYPE, ASSIGN_DETAIL, MANUAL_TASKS_SEQ, FINISHER_NAME_ID, FINISHER_NAME, ASSIGNER_ID, BRANCH_SEQ) 
-values(DAILY_TASKS_seq.nextval, null, '2018/05/08', 0, '파트', '오픈', 2, 'yunseok', '장윤석', 'yunyoung', 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>연진이 피카츄 생일케이크 사오기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>근무태만 반성문 작성해오기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김연진</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>개인</t>
-  </si>
-  <si>
-    <t>오픈</t>
-  </si>
-  <si>
-    <t>yunjin</t>
-  </si>
-  <si>
-    <t>미들</t>
-  </si>
-  <si>
-    <t>yunseok</t>
-  </si>
-  <si>
-    <t>장윤석</t>
-  </si>
-  <si>
-    <t>마감</t>
-  </si>
-  <si>
-    <t>taehun</t>
-  </si>
-  <si>
-    <t>김태훈</t>
   </si>
 </sst>
 </file>
@@ -2415,9 +2416,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2461,10 +2462,10 @@
         <v>114</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>128</v>
@@ -4326,16 +4327,16 @@
         <v>54</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="H56" s="1">
         <v>17</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>121</v>
@@ -4361,16 +4362,16 @@
         <v>54</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="H57" s="1">
         <v>12</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>121</v>
@@ -4384,7 +4385,7 @@
         <v>116</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>190</v>
@@ -4396,16 +4397,16 @@
         <v>54</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>121</v>
@@ -4431,16 +4432,16 @@
         <v>54</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="H59" s="1">
         <v>24</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>121</v>
@@ -4463,19 +4464,19 @@
         <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="H60" s="1">
         <v>21</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>121</v>
@@ -4501,16 +4502,16 @@
         <v>54</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="H61" s="1">
         <v>34</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>121</v>
@@ -4536,16 +4537,16 @@
         <v>54</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="H62" s="1">
         <v>19</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>121</v>
@@ -4571,16 +4572,16 @@
         <v>54</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="H63" s="1">
         <v>21</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>121</v>
@@ -4606,16 +4607,16 @@
         <v>54</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="H64" s="1">
         <v>19</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>121</v>
@@ -4641,16 +4642,16 @@
         <v>54</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="H65" s="1">
         <v>16</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>121</v>
@@ -4664,7 +4665,7 @@
         <v>116</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>190</v>
@@ -4676,16 +4677,16 @@
         <v>54</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>121</v>
@@ -4738,7 +4739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAFB34E-2FEC-4B7C-B013-1E0F4A147F5F}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -4757,152 +4758,152 @@
         <v>187</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B18" s="3" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B25" s="3" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B26" s="3" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B27" s="3" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B30" s="3" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="34" x14ac:dyDescent="0.45">
       <c r="B31" s="3" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
insert into staffs 코드 수정
</commit_message>
<xml_diff>
--- a/DB레코드.xlsx
+++ b/DB레코드.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B2CF414B-7AEC-4A28-9571-F8867A0EE604}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{483275D6-8D34-44F3-B77B-CD08CAF3F5BD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="3690" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1188,71 +1188,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'yunjin' , 'yunjin_resume.hwp' , 'yunjin_health.jpg' , 'yunjin_bank.png', '우리은행' , '1004427204842' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'heeeun' , 'heeeun_resume.hwp' , 'heeeun_health.jpg' , 'heeeun_bank.png' , '신한은행' , '110101764526' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'chanyoung' , 'chanyoung_resume.hwp' , 'chanyoung_health.jpg' , 'chanyoung_bank.png' , 'SC제일은행' , '10485675482' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'jonghyuk' , 'jonghyuk_resume.hwp' , 'jonghyuk_health.jpg' , 'jonghyuk_bank.png' , '하나은행' , '52546278031224' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'yunseok' , 'yunseok_resume.hwp' , 'yunseok_health.jpg' , 'yunseok_bank.png' , '신한은행' , '110468824651' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'taehun' , 'taehun_resume.hwp' , 'taehun_health.jpg' , null , '외환은행' , '336511098371' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'jaesun' , 'jaesun_resume.hwp' , 'jaesun_health.jpg' , null , 'NH농협은행' , '113478515465' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'yejee' , null , 'yejee_health.jpg' , null , '하나은행' , '98850424756733' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'hyesoo' , null , 'hyesoo_health.jpg' , null , '국민은행' , '42578500105462' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'jaemin' , null , 'jaemin_health.jpg' , null , '우리은행' , '1002546825713' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'eunkyul' , null , null , null , null , null , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'sumin' , null , null , 'sumin_bank.png' , null , null , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'seungkyun' , 'seungkyun_resume.hwp' , null , 'seungkyun_bank.png' , null , null , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'hyungjun' , 'hyungjun_resume.hwp' , null , 'hyungjun_bank.png' , null , null , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'chulsoo' , null , null , null , null , null , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'yeonghee' , 'yeonghee_resume.hwp' , null , 'yeonghee_bank.png' , null , null , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'minji' , 'minji_resume.hwp' , 'minji_health.jpg' , 'minji_bank.png' , '신한은행' , '113154209875' , 0 );</t>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'yunjin' , 'yunjin_resume.hwp' , 'yunjin_health.jpg' , 'yunjin_bank.png', '우리은행' , '1004427204842' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'heeeun' , 'heeeun_resume.hwp' , 'heeeun_health.jpg' , 'heeeun_bank.png' , '신한은행' , '110101764526' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'chanyoung' , 'chanyoung_resume.hwp' , 'chanyoung_health.jpg' , 'chanyoung_bank.png' , 'SC제일은행' , '10485675482' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'minji' , 'minji_resume.hwp' , 'minji_health.jpg' , 'minji_bank.png' , '신한은행' , '113154209875' , 0 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'yeonghee' , 'yeonghee_resume.hwp' , null , 'yeonghee_bank.png' , null , null , 0 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'chulsoo' , null , null , null , null , null , 0 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'hyungjun' , 'hyungjun_resume.hwp' , null , 'hyungjun_bank.png' , null , null , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'seungkyun' , 'seungkyun_resume.hwp' , null , 'seungkyun_bank.png' , null , null , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'sumin' , null , null , 'sumin_bank.png' , null , null , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'eunkyul' , null , null , null , null , null , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'jaemin' , null , 'jaemin_health.jpg' , null , '우리은행' , '1002546825713' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'hyesoo' , null , 'hyesoo_health.jpg' , null , '국민은행' , '42578500105462' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'yejee' , null , 'yejee_health.jpg' , null , '하나은행' , '98850424756733' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'jaesun' , 'jaesun_resume.hwp' , 'jaesun_health.jpg' , null , 'NH농협은행' , '113478515465' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'taehun' , 'taehun_resume.hwp' , 'taehun_health.jpg' , null , '외환은행' , '336511098371' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'yunseok' , 'yunseok_resume.hwp' , 'yunseok_health.jpg' , 'yunseok_bank.png' , '신한은행' , '110468824651' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'jonghyuk' , 'jonghyuk_resume.hwp' , 'jonghyuk_health.jpg' , 'jonghyuk_bank.png' , '하나은행' , '52546278031224' , 1 );</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5748,8 +5748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D6CD09-0CA1-42AC-AA82-9DE22EE2FD82}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5896,7 +5896,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>309</v>
+        <v>322</v>
       </c>
       <c r="K5" s="19"/>
     </row>
@@ -5923,7 +5923,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="K6" s="19"/>
     </row>
@@ -5950,7 +5950,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -5977,7 +5977,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="K8" s="19"/>
     </row>
@@ -6004,7 +6004,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="K9" s="19"/>
     </row>
@@ -6031,7 +6031,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="K10" s="19"/>
     </row>
@@ -6058,7 +6058,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="K11" s="19"/>
     </row>
@@ -6085,7 +6085,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K12" s="19"/>
     </row>
@@ -6112,7 +6112,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="K13" s="19"/>
     </row>
@@ -6139,7 +6139,7 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="K14" s="19"/>
     </row>
@@ -6166,7 +6166,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="K15" s="19"/>
     </row>
@@ -6193,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="K16" s="19"/>
     </row>
@@ -6220,7 +6220,7 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="K17" s="19"/>
     </row>
@@ -6247,7 +6247,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="K18" s="19"/>
     </row>

</xml_diff>

<commit_message>
admins DB insert용 - admins테이블 & users 테이블 추가
</commit_message>
<xml_diff>
--- a/DB레코드.xlsx
+++ b/DB레코드.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5AA01847-1F62-4C2E-BBC6-70C28C6E7089}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BED7147E-5B61-4CCF-8846-6784AE972CFC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="3690" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="3690" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="매뉴얼" sheetId="1" r:id="rId1"/>
@@ -1213,30 +1213,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'hyungjun' , 'hyungjun_resume.hwp' , null , 'hyungjun_bank.png' , null , null , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'seungkyun' , 'seungkyun_resume.hwp' , null , 'seungkyun_bank.png' , null , null , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'sumin' , null , null , 'sumin_bank.png' , null , null , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'eunkyul' , null , null , null , null , null , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'jaemin' , null , 'jaemin_health.jpg' , null , '우리은행' , '1002546825713' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'hyesoo' , null , 'hyesoo_health.jpg' , null , '국민은행' , '42578500105462' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'yejee' , null , 'yejee_health.jpg' , null , '하나은행' , '98850424756733' , 1 );</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1721,10 +1697,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'yeonghee' , 'yeonghee1234' , '01098561452' , '허영희' , '1989/03/21' , 'F' , 'yeonghee@naver.com' , '서울시' , '강북구' , '우이동' , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'yejee' , 'yejee1234' , '01020764174' , '이예지' , '1996/11/17' , 'F' , 'yejee@naver.com' , '서울시' , '동작구' , '상도동' , 1 );</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1741,10 +1713,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'minji' , 'minji1234' , '01051852547' , '김민지' , '1996/09/13' , 'F' , 'minji@naver.com' , '서울시' , '영등포구' , '여의도동' , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'jonghyuk' , 'jonghyuk1234' , '01020169206' , '박종혁' , '1996/05/12' , 'M' , 'jonghyuk@naver.com' , '서울시' , '마포구' , '공덕동' , 1 );</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1766,6 +1734,38 @@
   </si>
   <si>
     <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'heeeun' , 'heeeun1234' , '01072105321' , '강희은' , '1990/03/21' , 'F' , 'heeeun@naver.com' , '서울시' , '강서구' , '공항동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'hyesoo' , null , 'hyesoo_health.jpg' , null , '국민은행' , '42578500105462' , 2 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs (staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values ( 'jaemin' , null , 'jaemin_health.jpg' , null , '우리은행' , '1002546825713' , 2 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'eunkyul' , null , null , null , null , null , 2 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'sumin' , null , null , 'sumin_bank.png' , null , null , 2 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'seungkyun' , 'seungkyun_resume.hwp' , null , 'seungkyun_bank.png' , null , null , 2 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into staffs ( staff_id, resume_file, health_file, bank_file, bank_name, account_num, status ) values (  'hyungjun' , 'hyungjun_resume.hwp' , null , 'hyungjun_bank.png' , null , null , 2 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'minji' , 'minji1234' , '01051852547' , '김민지' , '1996/09/13' , 'F' , 'minji@naver.com' , '서울시' , '영등포구' , '여의도동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'yeonghee' , 'yeonghee1234' , '01098561452' , '허영희' , '1989/03/21' , 'F' , 'yeonghee@naver.com' , '서울시' , '강북구' , '우이동' , 1 );</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6277,8 +6277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D6CD09-0CA1-42AC-AA82-9DE22EE2FD82}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6425,7 +6425,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="K5" s="19"/>
     </row>
@@ -6452,7 +6452,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="K6" s="19"/>
     </row>
@@ -6479,7 +6479,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="K7" s="19"/>
     </row>
@@ -6506,7 +6506,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="K8" s="19"/>
     </row>
@@ -6533,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="K9" s="19"/>
     </row>
@@ -6557,10 +6557,10 @@
         <v>266</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>317</v>
+        <v>465</v>
       </c>
       <c r="K10" s="19"/>
     </row>
@@ -6584,10 +6584,10 @@
         <v>267</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>316</v>
+        <v>466</v>
       </c>
       <c r="K11" s="19"/>
     </row>
@@ -6611,10 +6611,10 @@
         <v>117</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>315</v>
+        <v>467</v>
       </c>
       <c r="K12" s="19"/>
     </row>
@@ -6638,10 +6638,10 @@
         <v>117</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>314</v>
+        <v>468</v>
       </c>
       <c r="K13" s="19"/>
     </row>
@@ -6665,10 +6665,10 @@
         <v>117</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>313</v>
+        <v>469</v>
       </c>
       <c r="K14" s="19"/>
     </row>
@@ -6692,10 +6692,10 @@
         <v>117</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J15" t="s">
-        <v>312</v>
+        <v>470</v>
       </c>
       <c r="K15" s="19"/>
     </row>
@@ -6792,7 +6792,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6811,34 +6811,34 @@
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="K1" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>331</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>332</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>238</v>
@@ -6846,82 +6846,82 @@
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B2" t="s">
         <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E2" t="s">
         <v>128</v>
       </c>
       <c r="F2" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="G2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>360</v>
+      </c>
+      <c r="I2" t="s">
+        <v>399</v>
+      </c>
+      <c r="J2" t="s">
         <v>400</v>
       </c>
-      <c r="H2" s="20" t="s">
-        <v>366</v>
-      </c>
-      <c r="I2" t="s">
-        <v>405</v>
-      </c>
-      <c r="J2" t="s">
-        <v>406</v>
-      </c>
       <c r="K2" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="O2" s="19"/>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C3" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="E3" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F3" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="G3" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="I3" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J3" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="K3" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="O3" s="19"/>
     </row>
@@ -6930,76 +6930,76 @@
         <v>247</v>
       </c>
       <c r="C4" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E4" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="F4" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="G4" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="I4" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="J4" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="K4" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="L4">
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="O4" s="19"/>
     </row>
     <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C5" t="s">
+        <v>380</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="E5" t="s">
         <v>335</v>
       </c>
-      <c r="C5" t="s">
-        <v>386</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>353</v>
-      </c>
-      <c r="E5" t="s">
-        <v>341</v>
-      </c>
       <c r="F5" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="G5" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="I5" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J5" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="K5" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="L5">
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="O5" s="19"/>
     </row>
@@ -7008,37 +7008,37 @@
         <v>245</v>
       </c>
       <c r="C6" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E6" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="F6" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="G6" t="s">
+        <v>398</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="I6" t="s">
         <v>404</v>
       </c>
-      <c r="H6" s="20" t="s">
-        <v>370</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
+        <v>409</v>
+      </c>
+      <c r="K6" t="s">
         <v>410</v>
-      </c>
-      <c r="J6" t="s">
-        <v>415</v>
-      </c>
-      <c r="K6" t="s">
-        <v>416</v>
       </c>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="O6" s="19"/>
     </row>
@@ -7047,37 +7047,37 @@
         <v>250</v>
       </c>
       <c r="C7" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E7" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="F7" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="G7" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="I7" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J7" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="K7" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="L7">
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="O7" s="19"/>
     </row>
@@ -7086,37 +7086,37 @@
         <v>246</v>
       </c>
       <c r="C8" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="E8" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F8" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="G8" t="s">
+        <v>398</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>366</v>
+      </c>
+      <c r="I8" t="s">
         <v>404</v>
       </c>
-      <c r="H8" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="I8" t="s">
-        <v>410</v>
-      </c>
       <c r="J8" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="K8" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="O8" s="19"/>
     </row>
@@ -7125,115 +7125,115 @@
         <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="E9" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="F9" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="G9" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="I9" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J9" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="K9" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="L9">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="O9" s="19"/>
     </row>
     <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C10" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="E10" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="F10" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="G10" t="s">
+        <v>394</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="I10" t="s">
+        <v>399</v>
+      </c>
+      <c r="J10" t="s">
         <v>400</v>
       </c>
-      <c r="H10" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="I10" t="s">
-        <v>405</v>
-      </c>
-      <c r="J10" t="s">
-        <v>406</v>
-      </c>
       <c r="K10" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="O10" s="19"/>
     </row>
     <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C11" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="E11" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="F11" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="G11" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="I11" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J11" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="K11" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="O11" s="19"/>
     </row>
@@ -7242,37 +7242,37 @@
         <v>249</v>
       </c>
       <c r="C12" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="E12" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="F12" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="G12" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="I12" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="J12" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="K12" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="O12" s="19"/>
     </row>
@@ -7281,37 +7281,37 @@
         <v>248</v>
       </c>
       <c r="C13" t="s">
+        <v>388</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="E13" t="s">
+        <v>343</v>
+      </c>
+      <c r="F13" t="s">
+        <v>444</v>
+      </c>
+      <c r="G13" t="s">
         <v>394</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>356</v>
-      </c>
-      <c r="E13" t="s">
-        <v>349</v>
-      </c>
-      <c r="F13" t="s">
-        <v>450</v>
-      </c>
-      <c r="G13" t="s">
-        <v>400</v>
-      </c>
       <c r="H13" s="20" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="I13" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="J13" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="K13" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="L13">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="O13" s="19"/>
     </row>
@@ -7320,37 +7320,37 @@
         <v>242</v>
       </c>
       <c r="C14" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E14" t="s">
         <v>130</v>
       </c>
       <c r="F14" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="G14" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="I14" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J14" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="K14" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="L14">
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="O14" s="19"/>
     </row>
@@ -7359,76 +7359,76 @@
         <v>244</v>
       </c>
       <c r="C15" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="E15" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="F15" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="G15" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="I15" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J15" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="K15" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="L15">
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="O15" s="19"/>
     </row>
     <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="C16" t="s">
+        <v>391</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>397</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>403</v>
-      </c>
       <c r="E16" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="F16" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="G16" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="I16" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J16" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="K16" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>461</v>
+        <v>472</v>
       </c>
       <c r="O16" s="19"/>
     </row>
@@ -7437,37 +7437,37 @@
         <v>240</v>
       </c>
       <c r="C17" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E17" t="s">
         <v>119</v>
       </c>
       <c r="F17" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="G17" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="I17" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J17" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="K17" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="O17" s="19"/>
     </row>
@@ -7476,37 +7476,37 @@
         <v>241</v>
       </c>
       <c r="C18" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E18" t="s">
         <v>129</v>
       </c>
       <c r="F18" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="G18" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="I18" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="J18" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="K18" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="L18">
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="O18" s="19"/>
     </row>

</xml_diff>

<commit_message>
admins & users 테이블 수정
</commit_message>
<xml_diff>
--- a/DB레코드.xlsx
+++ b/DB레코드.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2889775-220E-4EF5-9DB2-F5DA83FE68F3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3229D78F-B5E3-42F7-A10B-71D500197FE4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="3690" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="3690" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="매뉴얼" sheetId="1" r:id="rId1"/>
     <sheet name="일일업무" sheetId="2" r:id="rId2"/>
     <sheet name="일일업무 DB Insert용" sheetId="3" r:id="rId3"/>
     <sheet name="daily_tasks_query" sheetId="5" r:id="rId4"/>
-    <sheet name="직원인증정보 DB insert용" sheetId="6" r:id="rId5"/>
-    <sheet name="회원정보 DB insert용" sheetId="7" r:id="rId6"/>
+    <sheet name="staffs DB insert용" sheetId="6" r:id="rId5"/>
+    <sheet name="users DB insert용" sheetId="7" r:id="rId6"/>
     <sheet name="Admins DB insert용" sheetId="8" r:id="rId7"/>
     <sheet name="Branches DB insert용" sheetId="9" r:id="rId8"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="542">
   <si>
     <t>위생관리</t>
   </si>
@@ -1703,94 +1703,14 @@
     <t>'1992/11/20'</t>
   </si>
   <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'chulsoo' , 'chulsoo1234' , '01085239468' , '박철수' , '1992/07/24' , 'M' , 'chulsoo@naver.com' , '서울시' , '용산구' , '이촌동' , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'chanyoung' , 'chanyoung1234' , '01023606586' , '주찬영' , '1989/10/29' , 'M' , 'chanyoung@naver.com' , '서울시' , '마포구' , '도화동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'eunkyul' , 'eunkyul1234' , '01097291122' , '고은결' , '1991/09/04' , 'M' , 'eunkyul@naver.com' , '경기도' , '광명시' , '소하동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'yunseok' , 'yunseok1234' , '01099031063' , '장윤석' , '1992/11/20' , 'M' , 'yunseok@naver.com' , '서울시' , '송파구' , '석촌동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'yunjin' , 'yunjin1234' , '01053710710' , '김연진' , '1988/11/19' , 'F' , 'yunjin@naver.com' , '서울시' , '송파구' , '문정동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'yeonghee' , 'yeonghee1234' , '01098561452' , '허영희' , '1989/03/21' , 'F' , 'yeonghee@naver.com' , '서울시' , '강북구' , '우이동' , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'yejee' , 'yejee1234' , '01020764174' , '이예지' , '1996/11/17' , 'F' , 'yejee@naver.com' , '서울시' , '동작구' , '상도동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'taehun' , 'taehun1234' , '01032828507' , '김태훈' , '1998/05/30' , 'M' , 'taehun@naver.com' , '서울시' , '구로구' , '구로동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'sumin' , 'sumin1234' , '01025408580' , '박수민' , '1996/11/15' , 'M' ,' sumin@naver.com' , '경기도' , '수원시' , '매탄동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'seungkyun' , 'seungkyun1234' , '01098836283' , '함승균' , '1988/01/17' , 'M' , 'seungkyun@naver.com' , '경기도' , '오산시' , '가수동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'minji' , 'minji1234' , '01051852547' , '김민지' , '1996/09/13' , 'F' , 'minji@naver.com' , '서울시' , '영등포구' , '여의도동' , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'jonghyuk' , 'jonghyuk1234' , '01020169206' , '박종혁' , '1996/05/12' , 'M' , 'jonghyuk@naver.com' , '서울시' , '마포구' , '공덕동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'jaesun' , 'jaesun1234' ,'01094955647' , '이재선' , '1996/11/11' ,'M' , 'jaesun@naver.com' , '서울시' , '관악구' , '신림동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'jaemin' , 'jaemin1234' , '01093963130' , '최재민' , '1994/08/15' , 'F' , 'jaemin@naver.com' , '경기도' , '시흥시' , '정왕동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'hyungjun' , 'hyungjun1234' , '01040872442' , '민형준' , '1993/06/25' , 'M' , 'hyungjun@naver.com' , '서울시' , '강동구' , '상일동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'hyesoo' , 'hyesoo1234' , '01075794815' , '한혜수' , '1995/02/21' , 'F' , 'hyesoo@naver.com' , '경기도' , '과천시' , '과천동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'heeeun' , 'heeeun1234' , '01072105321' , '강희은' , '1990/03/21' , 'F' , 'heeeun@naver.com' , '서울시' , '강서구' , '공항동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into admins (admin_id, branch_seq, license_num, status) values ( 'hyeja' , branch_seq.nextval , '6018519876' , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hyeja</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into admins (admin_id, branch_seq, license_num, status) values ( 'minsu' , branch_seq.nextval , '1108554132' , 0 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>minsu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into admins (admin_id, branch_seq, license_num, status) values ( 'yunyoung' , branch_seq.nextval , '1008512345' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>license_num</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1835,10 +1755,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'yunyoung' , 'yunyoung1234' , '01085234512' , '홍윤영' , '1980/07/01' , 'F' , 'yunyoung@naver.com' , '서울시' , '서초구' ,  '방배동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>minsu1234</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1867,10 +1783,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'minsu' , 'minsu1234' , '01058428965' , '윤민수' , '1975/05/24' , 'M' , 'minsu@naver.com' , '서울시' , '송파구' , '문정동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>hyeja1234</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1903,10 +1815,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status) values ( 'hyeja' , 'hyeja1234' , '01063574821' , '김혜자' , '1971/04/05' , 'F' , 'hyeja@naver.com' , '부산광역시' , '해운대구' , '중1동' , 1 );</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>branch_name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1994,6 +1902,146 @@
   </si>
   <si>
     <t>insert into branches(branch_seq, branch_name, representative, branch_phone_num, opening_hour, address_city, address_gu, address_dong, address_detail) values ( branch_seq.nextval,  '가락시장점' , '홍윤영' , '0221574531' , '평일 08:00 ~ 23:00 / 주말 11:00 ~ 23:00' , '서울시' , '송파구' , '가락동' , '79-2 1층가락동' );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>profile_photo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chanyoung_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chulsoo_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yunyoung_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minsu_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'jonghyuk' , 'jonghyuk1234' , '01020169206' , '박종혁' , '1996/05/12' , 'M' , 'jonghyuk@naver.com' , '서울시' , '마포구' , '공덕동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'minji' , 'minji1234' , '01051852547' , '김민지' , '1996/09/13' , 'F' , 'minji@naver.com' , '서울시' , '영등포구' , '여의도동' , 0 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'seungkyun' , 'seungkyun1234' , '01098836283' , '함승균' , '1988/01/17' , 'M' , 'seungkyun@naver.com' , '경기도' , '오산시' , '가수동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'sumin' , 'sumin1234' , '01025408580' , '박수민' , '1996/11/15' , 'M' ,' sumin@naver.com' , '경기도' , '수원시' , '매탄동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'taehun' , 'taehun1234' , '01032828507' , '김태훈' , '1998/05/30' , 'M' , 'taehun@naver.com' , '서울시' , '구로구' , '구로동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'yejee' , 'yejee1234' , '01020764174' , '이예지' , '1996/11/17' , 'F' , 'yejee@naver.com' , '서울시' , '동작구' , '상도동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'yeonghee' , 'yeonghee1234' , '01098561452' , '허영희' , '1989/03/21' , 'F' , 'yeonghee@naver.com' , '서울시' , '강북구' , '우이동' , 0 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'yunjin' , 'yunjin1234' , '01053710710' , '김연진' , '1988/11/19' , 'F' , 'yunjin@naver.com' , '서울시' , '송파구' , '문정동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'yunseok' , 'yunseok1234' , '01099031063' , '장윤석' , '1992/11/20' , 'M' , 'yunseok@naver.com' , '서울시' , '송파구' , '석촌동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'hyeja' , 'hyeja1234' , '01063574821' , '김혜자' , '1971/04/05' , 'F' , 'hyeja@naver.com' , '부산광역시' , '해운대구' , '중1동' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'chanyoung' , 'chanyoung1234' , '01023606586' , '주찬영' , '1989/10/29' , 'M' , 'chanyoung@naver.com' , '서울시' , '마포구' , '도화동' , 1, 'chanyoung_profile.jpg' );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'chulsoo' , 'chulsoo1234' , '01085239468' , '박철수' , '1992/07/24' , 'M' , 'chulsoo@naver.com' , '서울시' , '용산구' , '이촌동' , 0 , 'chulsoo_profile.jpg');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eunkyul_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'eunkyul' , 'eunkyul1234' , '01097291122' , '고은결' , '1991/09/04' , 'M' , 'eunkyul@naver.com' , '경기도' , '광명시' , '소하동' , 1 , 'eunkyul_profile.jpg');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>heeeun_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'heeeun' , 'heeeun1234' , '01072105321' , '강희은' , '1990/03/21' , 'F' , 'heeeun@naver.com' , '서울시' , '강서구' , '공항동' , 1 ,'heeeun_profile.jpg');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hyesoo_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'hyesoo' , 'hyesoo1234' , '01075794815' , '한혜수' , '1995/02/21' , 'F' , 'hyesoo@naver.com' , '경기도' , '과천시' , '과천동' , 1 , 'hyesoo_profile.jpg');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hyungjun_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'hyungjun' , 'hyungjun1234' , '01040872442' , '민형준' , '1993/06/25' , 'M' , 'hyungjun@naver.com' , '서울시' , '강동구' , '상일동' , 1, 'hyungjun_profile.jpg');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jaemin_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'jaemin' , 'jaemin1234' , '01093963130' , '최재민' , '1994/08/15' , 'F' , 'jaemin@naver.com' , '경기도' , '시흥시' , '정왕동' , 1, 'jaemin_profile.jpg');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jaesun_profile.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'jaesun' , 'jaesun1234' ,'01094955647' , '이재선' , '1996/11/11' ,'M' , 'jaesun@naver.com' , '서울시' , '관악구' , '신림동' , 1, 'jaesun_profile.jpg' );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'yunyoung' , 'yunyoung1234' , '01085234512' , '홍윤영' , '1980/07/01' , 'F' , 'yunyoung@naver.com' , '서울시' , '서초구' ,  '방배동' , 1, 'yunyoung_profile.jpg');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'minsu' , 'minsu1234' , '01058428965' , '윤민수' , '1975/05/24' , 'M' , 'minsu@naver.com' , '서울시' , '송파구' , '문정동' , 1, 'minsu_profile.jpg');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into admins (admin_id, branch_seq, license_num, status) values ( 'yunyoung' , 1, '1008512345' , 1 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into admins (admin_id, branch_seq, license_num, status) values ( 'minsu' , 2 , '1108554132' , 0 );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into admins (admin_id, branch_seq, license_num, status) values ( 'hyeja' , 3, '6018519876' , 0 );</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6527,7 +6575,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7038,10 +7086,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9811FB-3469-427E-843F-58178652C230}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7055,10 +7103,11 @@
     <col min="7" max="7" width="5.75" customWidth="1"/>
     <col min="8" max="8" width="21.625" customWidth="1"/>
     <col min="9" max="11" width="11.375" customWidth="1"/>
-    <col min="14" max="14" width="120.875" customWidth="1"/>
+    <col min="13" max="13" width="19.125" customWidth="1"/>
+    <col min="15" max="15" width="120.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>323</v>
       </c>
@@ -7092,8 +7141,11 @@
       <c r="L1" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="4" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>333</v>
       </c>
@@ -7130,12 +7182,15 @@
       <c r="L2">
         <v>1</v>
       </c>
-      <c r="N2" t="s">
-        <v>457</v>
-      </c>
-      <c r="O2" s="19"/>
-    </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>508</v>
+      </c>
+      <c r="O2" t="s">
+        <v>523</v>
+      </c>
+      <c r="P2" s="19"/>
+    </row>
+    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>334</v>
       </c>
@@ -7169,12 +7224,15 @@
       <c r="L3">
         <v>0</v>
       </c>
-      <c r="N3" t="s">
-        <v>456</v>
-      </c>
-      <c r="O3" s="19"/>
-    </row>
-    <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>509</v>
+      </c>
+      <c r="O3" t="s">
+        <v>524</v>
+      </c>
+      <c r="P3" s="19"/>
+    </row>
+    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>247</v>
       </c>
@@ -7208,12 +7266,15 @@
       <c r="L4">
         <v>1</v>
       </c>
-      <c r="N4" t="s">
-        <v>458</v>
-      </c>
-      <c r="O4" s="19"/>
-    </row>
-    <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>525</v>
+      </c>
+      <c r="O4" t="s">
+        <v>526</v>
+      </c>
+      <c r="P4" s="19"/>
+    </row>
+    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>335</v>
       </c>
@@ -7247,12 +7308,15 @@
       <c r="L5">
         <v>1</v>
       </c>
-      <c r="N5" t="s">
-        <v>472</v>
-      </c>
-      <c r="O5" s="19"/>
-    </row>
-    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>527</v>
+      </c>
+      <c r="O5" t="s">
+        <v>528</v>
+      </c>
+      <c r="P5" s="19"/>
+    </row>
+    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>245</v>
       </c>
@@ -7286,12 +7350,15 @@
       <c r="L6">
         <v>1</v>
       </c>
-      <c r="N6" t="s">
-        <v>471</v>
-      </c>
-      <c r="O6" s="19"/>
-    </row>
-    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>529</v>
+      </c>
+      <c r="O6" t="s">
+        <v>530</v>
+      </c>
+      <c r="P6" s="19"/>
+    </row>
+    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>250</v>
       </c>
@@ -7325,12 +7392,15 @@
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="N7" t="s">
-        <v>470</v>
-      </c>
-      <c r="O7" s="19"/>
-    </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>531</v>
+      </c>
+      <c r="O7" t="s">
+        <v>532</v>
+      </c>
+      <c r="P7" s="19"/>
+    </row>
+    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>246</v>
       </c>
@@ -7364,12 +7434,15 @@
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="N8" t="s">
-        <v>469</v>
-      </c>
-      <c r="O8" s="19"/>
-    </row>
-    <row r="9" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>533</v>
+      </c>
+      <c r="O8" t="s">
+        <v>534</v>
+      </c>
+      <c r="P8" s="19"/>
+    </row>
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>243</v>
       </c>
@@ -7403,12 +7476,15 @@
       <c r="L9">
         <v>1</v>
       </c>
-      <c r="N9" t="s">
-        <v>468</v>
-      </c>
-      <c r="O9" s="19"/>
-    </row>
-    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>535</v>
+      </c>
+      <c r="O9" t="s">
+        <v>536</v>
+      </c>
+      <c r="P9" s="19"/>
+    </row>
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>336</v>
       </c>
@@ -7442,12 +7518,15 @@
       <c r="L10">
         <v>1</v>
       </c>
-      <c r="N10" t="s">
-        <v>467</v>
-      </c>
-      <c r="O10" s="19"/>
-    </row>
-    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>522</v>
+      </c>
+      <c r="O10" t="s">
+        <v>512</v>
+      </c>
+      <c r="P10" s="19"/>
+    </row>
+    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>337</v>
       </c>
@@ -7481,12 +7560,15 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="N11" t="s">
-        <v>466</v>
-      </c>
-      <c r="O11" s="19"/>
-    </row>
-    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>522</v>
+      </c>
+      <c r="O11" t="s">
+        <v>513</v>
+      </c>
+      <c r="P11" s="19"/>
+    </row>
+    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>249</v>
       </c>
@@ -7520,12 +7602,15 @@
       <c r="L12">
         <v>1</v>
       </c>
-      <c r="N12" t="s">
-        <v>465</v>
-      </c>
-      <c r="O12" s="19"/>
-    </row>
-    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>522</v>
+      </c>
+      <c r="O12" t="s">
+        <v>514</v>
+      </c>
+      <c r="P12" s="19"/>
+    </row>
+    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>248</v>
       </c>
@@ -7559,12 +7644,15 @@
       <c r="L13">
         <v>1</v>
       </c>
-      <c r="N13" t="s">
-        <v>464</v>
-      </c>
-      <c r="O13" s="19"/>
-    </row>
-    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>522</v>
+      </c>
+      <c r="O13" t="s">
+        <v>515</v>
+      </c>
+      <c r="P13" s="19"/>
+    </row>
+    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>242</v>
       </c>
@@ -7598,12 +7686,15 @@
       <c r="L14">
         <v>1</v>
       </c>
-      <c r="N14" t="s">
-        <v>463</v>
-      </c>
-      <c r="O14" s="19"/>
-    </row>
-    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>522</v>
+      </c>
+      <c r="O14" t="s">
+        <v>516</v>
+      </c>
+      <c r="P14" s="19"/>
+    </row>
+    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>244</v>
       </c>
@@ -7637,12 +7728,15 @@
       <c r="L15">
         <v>1</v>
       </c>
-      <c r="N15" t="s">
-        <v>462</v>
-      </c>
-      <c r="O15" s="19"/>
-    </row>
-    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M15" t="s">
+        <v>522</v>
+      </c>
+      <c r="O15" t="s">
+        <v>517</v>
+      </c>
+      <c r="P15" s="19"/>
+    </row>
+    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>338</v>
       </c>
@@ -7676,12 +7770,15 @@
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="N16" t="s">
-        <v>461</v>
-      </c>
-      <c r="O16" s="19"/>
-    </row>
-    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>522</v>
+      </c>
+      <c r="O16" t="s">
+        <v>518</v>
+      </c>
+      <c r="P16" s="19"/>
+    </row>
+    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>240</v>
       </c>
@@ -7715,12 +7812,15 @@
       <c r="L17">
         <v>1</v>
       </c>
-      <c r="N17" t="s">
-        <v>460</v>
-      </c>
-      <c r="O17" s="19"/>
-    </row>
-    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M17" t="s">
+        <v>522</v>
+      </c>
+      <c r="O17" t="s">
+        <v>519</v>
+      </c>
+      <c r="P17" s="19"/>
+    </row>
+    <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>241</v>
       </c>
@@ -7754,127 +7854,139 @@
       <c r="L18">
         <v>1</v>
       </c>
-      <c r="N18" t="s">
-        <v>459</v>
-      </c>
-      <c r="O18" s="19"/>
-    </row>
-    <row r="19" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M18" t="s">
+        <v>522</v>
+      </c>
+      <c r="O18" t="s">
+        <v>520</v>
+      </c>
+      <c r="P18" s="19"/>
+    </row>
+    <row r="19" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="B20" t="s">
         <v>120</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>481</v>
+        <v>461</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>482</v>
+        <v>462</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>484</v>
+        <v>464</v>
       </c>
       <c r="G20" t="s">
         <v>404</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>485</v>
+        <v>465</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>487</v>
+        <v>467</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>488</v>
+        <v>468</v>
       </c>
       <c r="L20" s="22">
         <v>1</v>
       </c>
-      <c r="N20" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M20" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="O20" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="G21" t="s">
         <v>400</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="K21" s="22" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="L21" s="22">
         <v>1</v>
       </c>
-      <c r="N21" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M21" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="O21" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>498</v>
+        <v>476</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>501</v>
+        <v>479</v>
       </c>
       <c r="G22" t="s">
         <v>404</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>502</v>
+        <v>480</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>504</v>
+        <v>482</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>505</v>
+        <v>483</v>
       </c>
       <c r="L22" s="22">
         <v>1</v>
       </c>
-      <c r="N22" t="s">
-        <v>506</v>
+      <c r="M22" s="22" t="s">
+        <v>522</v>
+      </c>
+      <c r="O22" t="s">
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -7909,8 +8021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D262D3F-58B4-43CE-A4C2-0BE7617B40B2}">
   <dimension ref="B1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7926,13 +8038,13 @@
   <sheetData>
     <row r="1" spans="2:7" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>479</v>
+        <v>459</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>115</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>238</v>
@@ -7952,12 +8064,12 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>477</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>476</v>
+        <v>457</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -7969,12 +8081,12 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>475</v>
+        <v>540</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>474</v>
+        <v>456</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7986,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>473</v>
+        <v>541</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -8002,8 +8114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67DE842B-8361-4A2D-9D9A-659B4B1BB3DA}">
   <dimension ref="B1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8025,16 +8137,16 @@
         <v>115</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>507</v>
+        <v>484</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>508</v>
+        <v>485</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>509</v>
+        <v>486</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>510</v>
+        <v>487</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>330</v>
@@ -8046,7 +8158,7 @@
         <v>332</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>511</v>
+        <v>488</v>
       </c>
     </row>
     <row r="2" spans="2:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
@@ -8054,31 +8166,31 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>512</v>
+        <v>489</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>483</v>
+        <v>463</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>516</v>
+        <v>493</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>518</v>
+        <v>495</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>525</v>
+        <v>502</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>526</v>
+        <v>503</v>
       </c>
       <c r="L2" t="s">
-        <v>529</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
@@ -8086,31 +8198,31 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>513</v>
+        <v>490</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>517</v>
+        <v>494</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>519</v>
+        <v>496</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>486</v>
+        <v>466</v>
       </c>
       <c r="H3" s="22" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>524</v>
+        <v>501</v>
       </c>
       <c r="L3" t="s">
-        <v>527</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -8118,31 +8230,31 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>514</v>
+        <v>491</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>515</v>
+        <v>492</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>520</v>
+        <v>497</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>503</v>
+        <v>481</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>504</v>
+        <v>482</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>521</v>
+        <v>498</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>522</v>
+        <v>499</v>
       </c>
       <c r="L4" t="s">
-        <v>528</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
DB레코드.xlsx에 staff_seq내용과 branch_staffs 추가
</commit_message>
<xml_diff>
--- a/DB레코드.xlsx
+++ b/DB레코드.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\workspace\Matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0CA158DA-F4D0-4845-992A-8489E4FAB282}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EFD7EBC3-BA7D-4BC1-B180-A097791CC05E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="3690" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15900" windowHeight="3690" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="매뉴얼" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="users DB insert용" sheetId="7" r:id="rId6"/>
     <sheet name="Admins DB insert용" sheetId="8" r:id="rId7"/>
     <sheet name="Branches DB insert용" sheetId="9" r:id="rId8"/>
+    <sheet name="Branch_staffs DB insert용" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">일일업무!$A$1:$D$35</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="601">
   <si>
     <t>위생관리</t>
   </si>
@@ -2042,6 +2043,190 @@
   </si>
   <si>
     <t>insert into users (user_id, pw, phone_num, name, birth, gender, email, address_city, address_gu, address_dong, status, profile_photo) values ( 'hyeja' , 'hyeja1234' , '01063574821' , '김혜자' , '1971/04/05' , 'F' , 'hyeja@naver.com' , '부산광역시' , '해운대구' , '중1동' , 1, null );</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2017/07/10', null, 1, 'heeeun', '오픈');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2018/01/19', null, 1, 'chanyoung', '미들');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2018/02/15', null, 1, 'jonghyuk', '미들');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2016/11/29', null, 1, 'yunseok', '미들');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2017/04/15', null, 1, 'taehun', '마감');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2016/12/07', null, 1, 'jaesun', '마감');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2018/01/26', null, 1, 'yejee', '마감');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2014/10/31', '2016/11/11', 1, 'hyesoo', '오픈');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2016/11/05', '2017/06/05', 1, 'jaemin', '오픈');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2015/05/13', '2016/12/03', 1, 'eunkyul', '미들');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2016/10/31', '2017/04/20', 1, 'sumin', '미들');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2016/08/10', '2017/04/18', 1, 'seungkyun', '마감');</t>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2015/03/17', '2016/12/30', 1, 'hyungjun', '마감');</t>
+  </si>
+  <si>
+    <t>branch_staffs_seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>join_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leave_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>work_part</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into branch_staffs (branch_staffs_seq, join_date, leave_date, branches_seq, staff_id, work_part) values(branch_staffs_seq.nextval, '2017/05/31', null, 1, 'yunjin', '오픈');</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2017/05/31'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> null</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'yunjin'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '오픈'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2017/07/10'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'heeeun'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2018/01/19'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'chanyoung'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '미들'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2018/02/15'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'jonghyuk'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2016/11/29'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'yunseok'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2017/04/15'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'taehun'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '마감'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2016/12/07'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'jaesun'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2018/01/26'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'yejee'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2014/10/31'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2016/11/11'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'hyesoo'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2016/11/05'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2017/06/05'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'jaemin'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2015/05/13'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2016/12/03'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'eunkyul'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2016/10/31'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2017/04/20'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'sumin'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2016/08/10'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2017/04/18'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'seungkyun'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2015/03/17'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '2016/12/30'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'hyungjun'</t>
+  </si>
+  <si>
+    <t>branch_staffs_seq.nextval</t>
+  </si>
+  <si>
+    <t>staff_seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>staff_seq.nextval</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2529,7 +2714,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3572,7 +3757,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
+      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5891,8 +6076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAFB34E-2FEC-4B7C-B013-1E0F4A147F5F}">
   <dimension ref="A1:B126"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -6572,329 +6757,363 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D6CD09-0CA1-42AC-AA82-9DE22EE2FD82}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="5" width="21.625" customWidth="1"/>
-    <col min="6" max="6" width="12.375" customWidth="1"/>
-    <col min="7" max="7" width="21.625" customWidth="1"/>
-    <col min="8" max="8" width="8.75" customWidth="1"/>
-    <col min="10" max="10" width="88.625" customWidth="1"/>
-    <col min="11" max="11" width="25.625" customWidth="1"/>
-    <col min="13" max="13" width="8.25" customWidth="1"/>
-    <col min="14" max="14" width="1.375" customWidth="1"/>
+    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="4" max="6" width="21.625" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
+    <col min="8" max="8" width="21.625" customWidth="1"/>
+    <col min="9" max="9" width="8.75" customWidth="1"/>
+    <col min="11" max="11" width="88.625" customWidth="1"/>
+    <col min="12" max="12" width="25.625" customWidth="1"/>
+    <col min="14" max="14" width="8.25" customWidth="1"/>
+    <col min="15" max="15" width="1.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>239</v>
       </c>
       <c r="B2" t="s">
+        <v>600</v>
+      </c>
+      <c r="C2" t="s">
         <v>240</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>273</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>285</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>284</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>251</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>258</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
         <v>306</v>
       </c>
-      <c r="K2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L2" s="19"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>600</v>
+      </c>
+      <c r="C3" t="s">
         <v>271</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>274</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>286</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>296</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>252</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>259</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>307</v>
       </c>
-      <c r="K3" s="19"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>600</v>
+      </c>
+      <c r="C4" t="s">
         <v>125</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>275</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>287</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>297</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>253</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>260</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
         <v>308</v>
       </c>
-      <c r="K4" s="19"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" s="19"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>600</v>
+      </c>
+      <c r="C5" t="s">
         <v>272</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>276</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>288</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>298</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>254</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>261</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
         <v>322</v>
       </c>
-      <c r="K5" s="19"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" s="19"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
+        <v>600</v>
+      </c>
+      <c r="C6" t="s">
         <v>241</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>277</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>289</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>299</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>252</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>262</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
         <v>321</v>
       </c>
-      <c r="K6" s="19"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" s="19"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>600</v>
+      </c>
+      <c r="C7" t="s">
         <v>242</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>278</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>290</v>
       </c>
-      <c r="E7" t="s">
-        <v>117</v>
-      </c>
       <c r="F7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" t="s">
         <v>256</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>263</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
         <v>320</v>
       </c>
-      <c r="K7" s="19"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
+        <v>600</v>
+      </c>
+      <c r="C8" t="s">
         <v>243</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>279</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>291</v>
       </c>
-      <c r="E8" t="s">
-        <v>117</v>
-      </c>
       <c r="F8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" t="s">
         <v>255</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>264</v>
       </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
         <v>319</v>
       </c>
-      <c r="K8" s="19"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>600</v>
+      </c>
+      <c r="C9" t="s">
         <v>244</v>
       </c>
-      <c r="C9" t="s">
-        <v>117</v>
-      </c>
       <c r="D9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" t="s">
         <v>292</v>
       </c>
-      <c r="E9" t="s">
-        <v>117</v>
-      </c>
       <c r="F9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" t="s">
         <v>254</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>265</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
         <v>318</v>
       </c>
-      <c r="K9" s="19"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>600</v>
+      </c>
+      <c r="C10" t="s">
         <v>245</v>
       </c>
-      <c r="C10" t="s">
-        <v>117</v>
-      </c>
       <c r="D10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" t="s">
         <v>293</v>
       </c>
-      <c r="E10" t="s">
-        <v>117</v>
-      </c>
       <c r="F10" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" t="s">
         <v>257</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>266</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
         <v>317</v>
       </c>
-      <c r="K10" s="19"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="19"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
+        <v>600</v>
+      </c>
+      <c r="C11" t="s">
         <v>246</v>
       </c>
-      <c r="C11" t="s">
-        <v>117</v>
-      </c>
       <c r="D11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" t="s">
         <v>294</v>
       </c>
-      <c r="E11" t="s">
-        <v>117</v>
-      </c>
       <c r="F11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" t="s">
         <v>251</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>267</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
         <v>316</v>
       </c>
-      <c r="K11" s="19"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>600</v>
+      </c>
+      <c r="C12" t="s">
         <v>247</v>
       </c>
-      <c r="C12" t="s">
-        <v>117</v>
-      </c>
       <c r="D12" t="s">
         <v>117</v>
       </c>
@@ -6907,102 +7126,114 @@
       <c r="G12" t="s">
         <v>117</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="H12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
         <v>315</v>
       </c>
-      <c r="K12" s="19"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>600</v>
+      </c>
+      <c r="C13" t="s">
         <v>248</v>
       </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
       <c r="D13" t="s">
         <v>117</v>
       </c>
       <c r="E13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" t="s">
         <v>300</v>
       </c>
-      <c r="F13" t="s">
-        <v>117</v>
-      </c>
       <c r="G13" t="s">
         <v>117</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="H13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13" t="s">
         <v>314</v>
       </c>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
+        <v>600</v>
+      </c>
+      <c r="C14" t="s">
         <v>249</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>280</v>
       </c>
-      <c r="D14" t="s">
-        <v>117</v>
-      </c>
       <c r="E14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" t="s">
         <v>301</v>
       </c>
-      <c r="F14" t="s">
-        <v>117</v>
-      </c>
       <c r="G14" t="s">
         <v>117</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="H14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
         <v>313</v>
       </c>
-      <c r="K14" s="19"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L14" s="19"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>600</v>
+      </c>
+      <c r="C15" t="s">
         <v>250</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>281</v>
       </c>
-      <c r="D15" t="s">
-        <v>117</v>
-      </c>
       <c r="E15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" t="s">
         <v>302</v>
       </c>
-      <c r="F15" t="s">
-        <v>117</v>
-      </c>
       <c r="G15" t="s">
         <v>117</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="H15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
         <v>312</v>
       </c>
-      <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>600</v>
+      </c>
+      <c r="C16" t="s">
         <v>268</v>
       </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
       <c r="D16" t="s">
         <v>117</v>
       </c>
@@ -7015,67 +7246,76 @@
       <c r="G16" t="s">
         <v>117</v>
       </c>
-      <c r="H16">
+      <c r="H16" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>311</v>
       </c>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
+        <v>600</v>
+      </c>
+      <c r="C17" t="s">
         <v>269</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>282</v>
       </c>
-      <c r="D17" t="s">
-        <v>117</v>
-      </c>
       <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
         <v>303</v>
       </c>
-      <c r="F17" t="s">
-        <v>117</v>
-      </c>
       <c r="G17" t="s">
         <v>117</v>
       </c>
-      <c r="H17">
+      <c r="H17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>310</v>
       </c>
-      <c r="K17" s="19"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>600</v>
+      </c>
+      <c r="C18" t="s">
         <v>270</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>283</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>295</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>304</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>252</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="H18" s="19" t="s">
         <v>305</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>309</v>
       </c>
-      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -7088,8 +7328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9811FB-3469-427E-843F-58178652C230}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8022,7 +8262,7 @@
   <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8115,7 +8355,7 @@
   <dimension ref="B1:L11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8264,4 +8504,419 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7595C9E6-A79D-43D7-8A7E-F7210DC4B33B}">
+  <dimension ref="B1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="5" max="6" width="20.125" customWidth="1"/>
+    <col min="7" max="7" width="13.25" customWidth="1"/>
+    <col min="8" max="8" width="14.625" customWidth="1"/>
+    <col min="9" max="9" width="5.5" customWidth="1"/>
+    <col min="10" max="10" width="11.75" customWidth="1"/>
+    <col min="11" max="12" width="10.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>598</v>
+      </c>
+      <c r="C2" t="s">
+        <v>560</v>
+      </c>
+      <c r="D2" t="s">
+        <v>561</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>562</v>
+      </c>
+      <c r="H2" t="s">
+        <v>563</v>
+      </c>
+      <c r="J2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>598</v>
+      </c>
+      <c r="C3" t="s">
+        <v>564</v>
+      </c>
+      <c r="D3" t="s">
+        <v>561</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>565</v>
+      </c>
+      <c r="H3" t="s">
+        <v>563</v>
+      </c>
+      <c r="J3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>598</v>
+      </c>
+      <c r="C4" t="s">
+        <v>566</v>
+      </c>
+      <c r="D4" t="s">
+        <v>561</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>567</v>
+      </c>
+      <c r="H4" t="s">
+        <v>568</v>
+      </c>
+      <c r="J4" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>598</v>
+      </c>
+      <c r="C5" t="s">
+        <v>569</v>
+      </c>
+      <c r="D5" t="s">
+        <v>561</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>570</v>
+      </c>
+      <c r="H5" t="s">
+        <v>568</v>
+      </c>
+      <c r="J5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>598</v>
+      </c>
+      <c r="C6" t="s">
+        <v>571</v>
+      </c>
+      <c r="D6" t="s">
+        <v>561</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>572</v>
+      </c>
+      <c r="H6" t="s">
+        <v>568</v>
+      </c>
+      <c r="J6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>598</v>
+      </c>
+      <c r="C7" t="s">
+        <v>573</v>
+      </c>
+      <c r="D7" t="s">
+        <v>561</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>574</v>
+      </c>
+      <c r="H7" t="s">
+        <v>575</v>
+      </c>
+      <c r="J7" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>598</v>
+      </c>
+      <c r="C8" t="s">
+        <v>576</v>
+      </c>
+      <c r="D8" t="s">
+        <v>561</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>577</v>
+      </c>
+      <c r="H8" t="s">
+        <v>575</v>
+      </c>
+      <c r="J8" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>598</v>
+      </c>
+      <c r="C9" t="s">
+        <v>578</v>
+      </c>
+      <c r="D9" t="s">
+        <v>561</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>579</v>
+      </c>
+      <c r="H9" t="s">
+        <v>575</v>
+      </c>
+      <c r="J9" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>598</v>
+      </c>
+      <c r="C10" t="s">
+        <v>580</v>
+      </c>
+      <c r="D10" t="s">
+        <v>581</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>582</v>
+      </c>
+      <c r="H10" t="s">
+        <v>563</v>
+      </c>
+      <c r="J10" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>598</v>
+      </c>
+      <c r="C11" t="s">
+        <v>583</v>
+      </c>
+      <c r="D11" t="s">
+        <v>584</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>585</v>
+      </c>
+      <c r="H11" t="s">
+        <v>563</v>
+      </c>
+      <c r="J11" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>598</v>
+      </c>
+      <c r="C12" t="s">
+        <v>586</v>
+      </c>
+      <c r="D12" t="s">
+        <v>587</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>588</v>
+      </c>
+      <c r="H12" t="s">
+        <v>568</v>
+      </c>
+      <c r="J12" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>598</v>
+      </c>
+      <c r="C13" t="s">
+        <v>589</v>
+      </c>
+      <c r="D13" t="s">
+        <v>590</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>591</v>
+      </c>
+      <c r="H13" t="s">
+        <v>568</v>
+      </c>
+      <c r="J13" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>598</v>
+      </c>
+      <c r="C14" t="s">
+        <v>592</v>
+      </c>
+      <c r="D14" t="s">
+        <v>593</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>594</v>
+      </c>
+      <c r="H14" t="s">
+        <v>575</v>
+      </c>
+      <c r="J14" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>598</v>
+      </c>
+      <c r="C15" t="s">
+        <v>595</v>
+      </c>
+      <c r="D15" t="s">
+        <v>596</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>597</v>
+      </c>
+      <c r="H15" t="s">
+        <v>575</v>
+      </c>
+      <c r="J15" t="s">
+        <v>554</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>